<commit_message>
Posters 2022 Ver 2
This is a model with 1 sigma for grades and a hierarchically determined grader variance.  It seems to work well. It needs to be retro-fitted to work on colab as well.
</commit_message>
<xml_diff>
--- a/tables posters 2022.xlsx
+++ b/tables posters 2022.xlsx
@@ -113,10 +113,10 @@
     <t>Judge 8</t>
   </si>
   <si>
+    <t>Judge 6</t>
+  </si>
+  <si>
     <t>Judge 17</t>
-  </si>
-  <si>
-    <t>Judge 6</t>
   </si>
   <si>
     <t>Judge 5</t>
@@ -614,7 +614,7 @@
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" customWidth="1"/>
@@ -720,7 +720,7 @@
         <v>27</v>
       </c>
       <c r="B2">
-        <v>-7.8</v>
+        <v>-6</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -735,7 +735,7 @@
         <v>89.3</v>
       </c>
       <c r="G2">
-        <v>95.8</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
         <v>52</v>
@@ -747,10 +747,10 @@
         <v>89</v>
       </c>
       <c r="K2">
-        <v>93.40000000000001</v>
+        <v>92</v>
       </c>
       <c r="L2">
-        <v>96.8</v>
+        <v>95</v>
       </c>
       <c r="M2" t="s">
         <v>50</v>
@@ -762,10 +762,10 @@
         <v>71</v>
       </c>
       <c r="P2">
-        <v>80.90000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="Q2">
-        <v>78.8</v>
+        <v>77</v>
       </c>
       <c r="R2" t="s">
         <v>64</v>
@@ -777,10 +777,10 @@
         <v>68</v>
       </c>
       <c r="U2">
-        <v>88.09999999999999</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="V2">
-        <v>75.8</v>
+        <v>74</v>
       </c>
       <c r="W2" t="s">
         <v>66</v>
@@ -792,10 +792,10 @@
         <v>83</v>
       </c>
       <c r="Z2">
-        <v>88.8</v>
+        <v>87.8</v>
       </c>
       <c r="AA2">
-        <v>90.8</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -803,7 +803,7 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>-6.8</v>
+        <v>-5.1</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -815,10 +815,10 @@
         <v>71</v>
       </c>
       <c r="F3">
-        <v>81.5</v>
+        <v>82.3</v>
       </c>
       <c r="G3">
-        <v>77.8</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
@@ -830,10 +830,10 @@
         <v>89</v>
       </c>
       <c r="K3">
-        <v>93.5</v>
+        <v>93.7</v>
       </c>
       <c r="L3">
-        <v>95.8</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="M3" t="s">
         <v>60</v>
@@ -845,10 +845,10 @@
         <v>82</v>
       </c>
       <c r="P3">
-        <v>89.7</v>
+        <v>90.2</v>
       </c>
       <c r="Q3">
-        <v>88.8</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="R3" t="s">
         <v>65</v>
@@ -886,7 +886,7 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <v>-5.9</v>
+        <v>-3.7</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
@@ -898,10 +898,10 @@
         <v>79</v>
       </c>
       <c r="F4">
-        <v>92.40000000000001</v>
+        <v>91.2</v>
       </c>
       <c r="G4">
-        <v>84.90000000000001</v>
+        <v>82.7</v>
       </c>
       <c r="H4" t="s">
         <v>54</v>
@@ -913,10 +913,10 @@
         <v>82</v>
       </c>
       <c r="K4">
-        <v>83.5</v>
+        <v>82.5</v>
       </c>
       <c r="L4">
-        <v>87.90000000000001</v>
+        <v>85.7</v>
       </c>
       <c r="M4" t="s">
         <v>52</v>
@@ -928,10 +928,10 @@
         <v>86</v>
       </c>
       <c r="P4">
-        <v>93.40000000000001</v>
+        <v>92</v>
       </c>
       <c r="Q4">
-        <v>91.90000000000001</v>
+        <v>89.7</v>
       </c>
       <c r="R4" t="s">
         <v>58</v>
@@ -943,10 +943,10 @@
         <v>90</v>
       </c>
       <c r="U4">
-        <v>89.7</v>
+        <v>89.8</v>
       </c>
       <c r="V4">
-        <v>95.90000000000001</v>
+        <v>93.7</v>
       </c>
       <c r="W4" t="s">
         <v>66</v>
@@ -958,10 +958,10 @@
         <v>79</v>
       </c>
       <c r="Z4">
-        <v>88.8</v>
+        <v>87.8</v>
       </c>
       <c r="AA4">
-        <v>84.90000000000001</v>
+        <v>82.7</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -969,7 +969,7 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>-4.9</v>
+        <v>-3.4</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -981,10 +981,10 @@
         <v>97</v>
       </c>
       <c r="F5">
-        <v>98.09999999999999</v>
+        <v>97.3</v>
       </c>
       <c r="G5">
-        <v>101.9</v>
+        <v>100.4</v>
       </c>
       <c r="H5" t="s">
         <v>55</v>
@@ -999,7 +999,7 @@
         <v>93</v>
       </c>
       <c r="L5">
-        <v>94.90000000000001</v>
+        <v>93.40000000000001</v>
       </c>
       <c r="M5" t="s">
         <v>51</v>
@@ -1011,10 +1011,10 @@
         <v>77</v>
       </c>
       <c r="P5">
-        <v>78.2</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="Q5">
-        <v>81.90000000000001</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="R5" t="s">
         <v>63</v>
@@ -1026,10 +1026,10 @@
         <v>64</v>
       </c>
       <c r="U5">
-        <v>79.90000000000001</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="V5">
-        <v>68.90000000000001</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="W5" t="s">
         <v>65</v>
@@ -1052,7 +1052,7 @@
         <v>31</v>
       </c>
       <c r="B6">
-        <v>-4.3</v>
+        <v>-2.5</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -1064,10 +1064,10 @@
         <v>89</v>
       </c>
       <c r="F6">
-        <v>92.40000000000001</v>
+        <v>91.2</v>
       </c>
       <c r="G6">
-        <v>93.3</v>
+        <v>91.5</v>
       </c>
       <c r="H6" t="s">
         <v>56</v>
@@ -1079,10 +1079,10 @@
         <v>90</v>
       </c>
       <c r="K6">
+        <v>92.40000000000001</v>
+      </c>
+      <c r="L6">
         <v>92.5</v>
-      </c>
-      <c r="L6">
-        <v>94.3</v>
       </c>
       <c r="M6" t="s">
         <v>54</v>
@@ -1094,10 +1094,10 @@
         <v>72</v>
       </c>
       <c r="P6">
-        <v>83.5</v>
+        <v>82.5</v>
       </c>
       <c r="Q6">
-        <v>76.3</v>
+        <v>74.5</v>
       </c>
       <c r="R6" t="s">
         <v>57</v>
@@ -1109,10 +1109,10 @@
         <v>77</v>
       </c>
       <c r="U6">
-        <v>78.3</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="V6">
-        <v>81.3</v>
+        <v>79.5</v>
       </c>
       <c r="W6" t="s">
         <v>65</v>
@@ -1135,67 +1135,67 @@
         <v>32</v>
       </c>
       <c r="B7">
-        <v>-1.2</v>
+        <v>-0.6</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7">
-        <v>97</v>
+        <v>93.3</v>
       </c>
       <c r="E7">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F7">
-        <v>98.09999999999999</v>
+        <v>92.7</v>
       </c>
       <c r="G7">
-        <v>95.2</v>
+        <v>92.59999999999999</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I7">
+        <v>76.3</v>
+      </c>
+      <c r="J7">
+        <v>74</v>
+      </c>
+      <c r="K7">
+        <v>78.09999999999999</v>
+      </c>
+      <c r="L7">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7">
         <v>89</v>
-      </c>
-      <c r="J7">
-        <v>92</v>
-      </c>
-      <c r="K7">
-        <v>93.40000000000001</v>
-      </c>
-      <c r="L7">
-        <v>93.2</v>
-      </c>
-      <c r="M7" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7">
-        <v>87.7</v>
       </c>
       <c r="O7">
         <v>84</v>
       </c>
       <c r="P7">
-        <v>85.90000000000001</v>
+        <v>87.8</v>
       </c>
       <c r="Q7">
-        <v>85.2</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="R7" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="S7">
-        <v>93.3</v>
+        <v>93.7</v>
       </c>
       <c r="T7">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="U7">
-        <v>92.7</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="V7">
-        <v>96.2</v>
+        <v>97.59999999999999</v>
       </c>
       <c r="W7" t="s">
         <v>65</v>
@@ -1218,67 +1218,67 @@
         <v>33</v>
       </c>
       <c r="B8">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8">
-        <v>93.3</v>
+        <v>97</v>
       </c>
       <c r="E8">
+        <v>94</v>
+      </c>
+      <c r="F8">
+        <v>97.3</v>
+      </c>
+      <c r="G8">
+        <v>94.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8">
+        <v>89</v>
+      </c>
+      <c r="J8">
         <v>92</v>
       </c>
-      <c r="F8">
-        <v>92.7</v>
-      </c>
-      <c r="G8">
-        <v>92.59999999999999</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8">
-        <v>76.3</v>
-      </c>
-      <c r="J8">
-        <v>74</v>
-      </c>
       <c r="K8">
-        <v>78.3</v>
+        <v>92</v>
       </c>
       <c r="L8">
-        <v>74.59999999999999</v>
+        <v>92.5</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N8">
-        <v>89</v>
+        <v>87.7</v>
       </c>
       <c r="O8">
         <v>84</v>
       </c>
       <c r="P8">
-        <v>86.90000000000001</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="Q8">
-        <v>84.59999999999999</v>
+        <v>84.5</v>
       </c>
       <c r="R8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="S8">
-        <v>93.7</v>
+        <v>93.3</v>
       </c>
       <c r="T8">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U8">
-        <v>91.90000000000001</v>
+        <v>92.7</v>
       </c>
       <c r="V8">
-        <v>97.59999999999999</v>
+        <v>95.5</v>
       </c>
       <c r="W8" t="s">
         <v>65</v>
@@ -1301,7 +1301,7 @@
         <v>34</v>
       </c>
       <c r="B9">
-        <v>-0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -1313,10 +1313,10 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>98.09999999999999</v>
+        <v>97.3</v>
       </c>
       <c r="G9">
-        <v>100.5</v>
+        <v>100.4</v>
       </c>
       <c r="H9" t="s">
         <v>45</v>
@@ -1328,10 +1328,10 @@
         <v>100</v>
       </c>
       <c r="K9">
-        <v>92.40000000000001</v>
+        <v>91.2</v>
       </c>
       <c r="L9">
-        <v>100.5</v>
+        <v>100.4</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
@@ -1343,10 +1343,10 @@
         <v>68</v>
       </c>
       <c r="P9">
-        <v>78.2</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="Q9">
-        <v>68.5</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="R9" t="s">
         <v>62</v>
@@ -1358,10 +1358,10 @@
         <v>87</v>
       </c>
       <c r="U9">
-        <v>91.90000000000001</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="V9">
-        <v>87.5</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="W9" t="s">
         <v>49</v>
@@ -1373,10 +1373,10 @@
         <v>92</v>
       </c>
       <c r="Z9">
-        <v>89.3</v>
+        <v>90.5</v>
       </c>
       <c r="AA9">
-        <v>92.5</v>
+        <v>92.40000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1384,7 +1384,7 @@
         <v>35</v>
       </c>
       <c r="B10">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
@@ -1396,10 +1396,10 @@
         <v>88</v>
       </c>
       <c r="F10">
-        <v>88.90000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="G10">
-        <v>87.2</v>
+        <v>87.8</v>
       </c>
       <c r="H10" t="s">
         <v>58</v>
@@ -1411,10 +1411,10 @@
         <v>85</v>
       </c>
       <c r="K10">
-        <v>89.7</v>
+        <v>89.8</v>
       </c>
       <c r="L10">
-        <v>84.2</v>
+        <v>84.8</v>
       </c>
       <c r="M10" t="s">
         <v>61</v>
@@ -1426,10 +1426,10 @@
         <v>87</v>
       </c>
       <c r="P10">
-        <v>85.90000000000001</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="Q10">
-        <v>86.2</v>
+        <v>86.8</v>
       </c>
       <c r="R10" t="s">
         <v>64</v>
@@ -1441,10 +1441,10 @@
         <v>96</v>
       </c>
       <c r="U10">
-        <v>88.09999999999999</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="V10">
-        <v>95.2</v>
+        <v>95.8</v>
       </c>
       <c r="W10" t="s">
         <v>65</v>
@@ -1467,7 +1467,7 @@
         <v>36</v>
       </c>
       <c r="B11">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>43</v>
@@ -1482,7 +1482,7 @@
         <v>89.3</v>
       </c>
       <c r="G11">
-        <v>86.7</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
         <v>55</v>
@@ -1497,7 +1497,7 @@
         <v>93</v>
       </c>
       <c r="L11">
-        <v>94.7</v>
+        <v>95</v>
       </c>
       <c r="M11" t="s">
         <v>56</v>
@@ -1509,10 +1509,10 @@
         <v>93</v>
       </c>
       <c r="P11">
-        <v>92.5</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="Q11">
-        <v>91.7</v>
+        <v>92</v>
       </c>
       <c r="R11" t="s">
         <v>54</v>
@@ -1524,10 +1524,10 @@
         <v>86</v>
       </c>
       <c r="U11">
-        <v>83.5</v>
+        <v>82.5</v>
       </c>
       <c r="V11">
-        <v>84.7</v>
+        <v>85</v>
       </c>
       <c r="W11" t="s">
         <v>53</v>
@@ -1539,10 +1539,10 @@
         <v>96</v>
       </c>
       <c r="Z11">
-        <v>93.5</v>
+        <v>93.7</v>
       </c>
       <c r="AA11">
-        <v>94.7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1550,7 +1550,7 @@
         <v>37</v>
       </c>
       <c r="B12">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -1565,7 +1565,7 @@
         <v>92.7</v>
       </c>
       <c r="G12">
-        <v>90.90000000000001</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H12" t="s">
         <v>57</v>
@@ -1577,10 +1577,10 @@
         <v>78</v>
       </c>
       <c r="K12">
-        <v>78.3</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="L12">
-        <v>75.90000000000001</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="M12" t="s">
         <v>59</v>
@@ -1592,10 +1592,10 @@
         <v>92</v>
       </c>
       <c r="P12">
-        <v>86.90000000000001</v>
+        <v>87.8</v>
       </c>
       <c r="Q12">
-        <v>89.90000000000001</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="R12" t="s">
         <v>66</v>
@@ -1607,10 +1607,10 @@
         <v>93</v>
       </c>
       <c r="U12">
-        <v>88.8</v>
+        <v>87.8</v>
       </c>
       <c r="V12">
-        <v>90.90000000000001</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="W12" t="s">
         <v>65</v>
@@ -1633,7 +1633,7 @@
         <v>38</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
@@ -1648,7 +1648,7 @@
         <v>89.3</v>
       </c>
       <c r="G13">
-        <v>86</v>
+        <v>87.3</v>
       </c>
       <c r="H13" t="s">
         <v>55</v>
@@ -1663,7 +1663,7 @@
         <v>93</v>
       </c>
       <c r="L13">
-        <v>91</v>
+        <v>92.3</v>
       </c>
       <c r="M13" t="s">
         <v>56</v>
@@ -1675,10 +1675,10 @@
         <v>97</v>
       </c>
       <c r="P13">
-        <v>92.5</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="Q13">
-        <v>93</v>
+        <v>94.3</v>
       </c>
       <c r="R13" t="s">
         <v>63</v>
@@ -1690,10 +1690,10 @@
         <v>90</v>
       </c>
       <c r="U13">
-        <v>79.90000000000001</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="V13">
-        <v>86</v>
+        <v>87.3</v>
       </c>
       <c r="W13" t="s">
         <v>60</v>
@@ -1705,10 +1705,10 @@
         <v>94</v>
       </c>
       <c r="Z13">
-        <v>89.7</v>
+        <v>90.2</v>
       </c>
       <c r="AA13">
-        <v>90</v>
+        <v>91.3</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1716,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>2.8</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
@@ -1728,10 +1728,10 @@
         <v>94</v>
       </c>
       <c r="F14">
-        <v>89.3</v>
+        <v>90.5</v>
       </c>
       <c r="G14">
-        <v>89</v>
+        <v>91.2</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
@@ -1743,10 +1743,10 @@
         <v>90</v>
       </c>
       <c r="K14">
-        <v>81.5</v>
+        <v>82.3</v>
       </c>
       <c r="L14">
-        <v>85</v>
+        <v>87.2</v>
       </c>
       <c r="M14" t="s">
         <v>53</v>
@@ -1758,10 +1758,10 @@
         <v>97</v>
       </c>
       <c r="P14">
-        <v>93.5</v>
+        <v>93.7</v>
       </c>
       <c r="Q14">
-        <v>92</v>
+        <v>94.2</v>
       </c>
       <c r="R14" t="s">
         <v>65</v>
@@ -1799,7 +1799,7 @@
         <v>40</v>
       </c>
       <c r="B15">
-        <v>5.1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
@@ -1811,10 +1811,10 @@
         <v>98</v>
       </c>
       <c r="F15">
-        <v>88.90000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="G15">
-        <v>92.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
         <v>59</v>
@@ -1826,10 +1826,10 @@
         <v>91</v>
       </c>
       <c r="K15">
-        <v>86.90000000000001</v>
+        <v>87.8</v>
       </c>
       <c r="L15">
-        <v>85.90000000000001</v>
+        <v>88</v>
       </c>
       <c r="M15" t="s">
         <v>62</v>
@@ -1841,10 +1841,10 @@
         <v>97</v>
       </c>
       <c r="P15">
-        <v>91.90000000000001</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="Q15">
-        <v>91.90000000000001</v>
+        <v>94</v>
       </c>
       <c r="R15" t="s">
         <v>49</v>
@@ -1856,10 +1856,10 @@
         <v>92</v>
       </c>
       <c r="U15">
-        <v>89.3</v>
+        <v>90.5</v>
       </c>
       <c r="V15">
-        <v>86.90000000000001</v>
+        <v>89</v>
       </c>
       <c r="W15" t="s">
         <v>60</v>
@@ -1871,10 +1871,10 @@
         <v>96</v>
       </c>
       <c r="Z15">
-        <v>89.7</v>
+        <v>90.2</v>
       </c>
       <c r="AA15">
-        <v>90.90000000000001</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1882,7 +1882,7 @@
         <v>41</v>
       </c>
       <c r="B16">
-        <v>6.6</v>
+        <v>4.6</v>
       </c>
       <c r="C16" t="s">
         <v>50</v>
@@ -1894,10 +1894,10 @@
         <v>87</v>
       </c>
       <c r="F16">
-        <v>80.90000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="G16">
-        <v>80.40000000000001</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>58</v>
@@ -1909,10 +1909,10 @@
         <v>96</v>
       </c>
       <c r="K16">
-        <v>89.7</v>
+        <v>89.8</v>
       </c>
       <c r="L16">
-        <v>89.40000000000001</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="M16" t="s">
         <v>61</v>
@@ -1924,10 +1924,10 @@
         <v>92</v>
       </c>
       <c r="P16">
-        <v>85.90000000000001</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="Q16">
-        <v>85.40000000000001</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="R16" t="s">
         <v>64</v>
@@ -1939,10 +1939,10 @@
         <v>100</v>
       </c>
       <c r="U16">
-        <v>88.09999999999999</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="V16">
-        <v>93.40000000000001</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="W16" t="s">
         <v>44</v>
@@ -1954,10 +1954,10 @@
         <v>86</v>
       </c>
       <c r="Z16">
-        <v>81.5</v>
+        <v>82.3</v>
       </c>
       <c r="AA16">
-        <v>79.40000000000001</v>
+        <v>81.40000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1965,7 +1965,7 @@
         <v>42</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>7.4</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -1977,10 +1977,10 @@
         <v>91</v>
       </c>
       <c r="F17">
-        <v>78.2</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="G17">
-        <v>81</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="H17" t="s">
         <v>50</v>
@@ -1992,10 +1992,10 @@
         <v>91</v>
       </c>
       <c r="K17">
-        <v>80.90000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="L17">
-        <v>81</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="M17" t="s">
         <v>63</v>
@@ -2007,10 +2007,10 @@
         <v>92</v>
       </c>
       <c r="P17">
-        <v>79.90000000000001</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="Q17">
-        <v>82</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="R17" t="s">
         <v>48</v>
@@ -2022,10 +2022,10 @@
         <v>97</v>
       </c>
       <c r="U17">
-        <v>88.90000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="V17">
-        <v>87</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="W17" t="s">
         <v>65</v>
@@ -2059,18 +2059,18 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2122,96 +2122,96 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B2">
-        <v>78.7</v>
+        <v>76.3</v>
       </c>
       <c r="C2">
-        <v>78.2</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="D2">
-        <v>-0.5</v>
+        <v>1.8</v>
       </c>
       <c r="E2">
-        <v>77.09999999999999</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="F2">
-        <v>-1.5</v>
+        <v>0.6</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2">
         <v>77</v>
       </c>
       <c r="I2">
-        <v>81.90000000000001</v>
+        <v>79.5</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K2">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="L2">
-        <v>68.5</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="O2">
-        <v>81</v>
+        <v>76.59999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3">
-        <v>76.3</v>
+        <v>78.7</v>
       </c>
       <c r="C3">
-        <v>78.3</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>-0</v>
       </c>
       <c r="E3">
-        <v>77.3</v>
+        <v>77.5</v>
       </c>
       <c r="F3">
-        <v>0.9</v>
+        <v>-1.2</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>77</v>
       </c>
       <c r="I3">
-        <v>81.3</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K3">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L3">
-        <v>74.59999999999999</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="N3">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="O3">
-        <v>75.90000000000001</v>
+        <v>83.59999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2222,16 +2222,16 @@
         <v>82</v>
       </c>
       <c r="C4">
-        <v>79.90000000000001</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="D4">
-        <v>-2.1</v>
+        <v>-1.4</v>
       </c>
       <c r="E4">
-        <v>78.90000000000001</v>
+        <v>79.8</v>
       </c>
       <c r="F4">
-        <v>-3.1</v>
+        <v>-2.2</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
@@ -2240,7 +2240,7 @@
         <v>64</v>
       </c>
       <c r="I4">
-        <v>68.90000000000001</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
@@ -2249,7 +2249,7 @@
         <v>90</v>
       </c>
       <c r="L4">
-        <v>86</v>
+        <v>87.3</v>
       </c>
       <c r="M4" t="s">
         <v>42</v>
@@ -2258,7 +2258,7 @@
         <v>92</v>
       </c>
       <c r="O4">
-        <v>82</v>
+        <v>84.59999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2269,16 +2269,16 @@
         <v>83</v>
       </c>
       <c r="C5">
-        <v>80.90000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="D5">
-        <v>-2.1</v>
+        <v>-1.2</v>
       </c>
       <c r="E5">
-        <v>80.09999999999999</v>
+        <v>81</v>
       </c>
       <c r="F5">
-        <v>-2.9</v>
+        <v>-2</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -2287,7 +2287,7 @@
         <v>71</v>
       </c>
       <c r="I5">
-        <v>78.8</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
         <v>42</v>
@@ -2296,7 +2296,7 @@
         <v>91</v>
       </c>
       <c r="L5">
-        <v>81</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="M5" t="s">
         <v>41</v>
@@ -2305,7 +2305,7 @@
         <v>87</v>
       </c>
       <c r="O5">
-        <v>80.40000000000001</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2316,16 +2316,16 @@
         <v>82.3</v>
       </c>
       <c r="C6">
-        <v>81.5</v>
+        <v>82.3</v>
       </c>
       <c r="D6">
-        <v>-0.9</v>
+        <v>-0.1</v>
       </c>
       <c r="E6">
-        <v>80.7</v>
+        <v>81.59999999999999</v>
       </c>
       <c r="F6">
-        <v>-1.6</v>
+        <v>-0.7</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
@@ -2334,7 +2334,7 @@
         <v>71</v>
       </c>
       <c r="I6">
-        <v>77.8</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="J6" t="s">
         <v>39</v>
@@ -2343,7 +2343,7 @@
         <v>90</v>
       </c>
       <c r="L6">
-        <v>85</v>
+        <v>87.2</v>
       </c>
       <c r="M6" t="s">
         <v>41</v>
@@ -2352,7 +2352,7 @@
         <v>86</v>
       </c>
       <c r="O6">
-        <v>79.40000000000001</v>
+        <v>81.40000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2363,16 +2363,16 @@
         <v>80</v>
       </c>
       <c r="C7">
-        <v>83.5</v>
+        <v>82.5</v>
       </c>
       <c r="D7">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="E7">
-        <v>83</v>
+        <v>81.8</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>1.8</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -2381,7 +2381,7 @@
         <v>72</v>
       </c>
       <c r="I7">
-        <v>76.3</v>
+        <v>74.5</v>
       </c>
       <c r="J7" t="s">
         <v>36</v>
@@ -2390,7 +2390,7 @@
         <v>86</v>
       </c>
       <c r="L7">
-        <v>84.7</v>
+        <v>85</v>
       </c>
       <c r="M7" t="s">
         <v>29</v>
@@ -2399,7 +2399,7 @@
         <v>82</v>
       </c>
       <c r="O7">
-        <v>87.90000000000001</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2410,16 +2410,16 @@
         <v>87.7</v>
       </c>
       <c r="C8">
-        <v>85.90000000000001</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="D8">
-        <v>-1.8</v>
+        <v>-1.3</v>
       </c>
       <c r="E8">
-        <v>85.59999999999999</v>
+        <v>86.2</v>
       </c>
       <c r="F8">
-        <v>-2.1</v>
+        <v>-1.4</v>
       </c>
       <c r="G8" t="s">
         <v>41</v>
@@ -2428,7 +2428,7 @@
         <v>92</v>
       </c>
       <c r="I8">
-        <v>85.40000000000001</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="J8" t="s">
         <v>35</v>
@@ -2437,16 +2437,16 @@
         <v>87</v>
       </c>
       <c r="L8">
-        <v>86.2</v>
+        <v>86.8</v>
       </c>
       <c r="M8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N8">
         <v>84</v>
       </c>
       <c r="O8">
-        <v>85.2</v>
+        <v>84.5</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2457,16 +2457,16 @@
         <v>89</v>
       </c>
       <c r="C9">
-        <v>86.90000000000001</v>
+        <v>87.8</v>
       </c>
       <c r="D9">
-        <v>-2.1</v>
+        <v>-1.2</v>
       </c>
       <c r="E9">
-        <v>86.8</v>
+        <v>87.7</v>
       </c>
       <c r="F9">
-        <v>-2.2</v>
+        <v>-1.3</v>
       </c>
       <c r="G9" t="s">
         <v>40</v>
@@ -2475,10 +2475,10 @@
         <v>91</v>
       </c>
       <c r="I9">
-        <v>85.90000000000001</v>
+        <v>88</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K9">
         <v>84</v>
@@ -2493,618 +2493,618 @@
         <v>92</v>
       </c>
       <c r="O9">
-        <v>89.90000000000001</v>
+        <v>90.59999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C10">
-        <v>88.09999999999999</v>
+        <v>87.8</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>2.8</v>
       </c>
       <c r="E10">
-        <v>88.09999999999999</v>
+        <v>87.8</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>2.8</v>
       </c>
       <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <v>79</v>
+      </c>
+      <c r="I10">
+        <v>82.7</v>
+      </c>
+      <c r="J10" t="s">
         <v>27</v>
       </c>
-      <c r="H10">
-        <v>68</v>
-      </c>
-      <c r="I10">
-        <v>75.8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
-      </c>
       <c r="K10">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="L10">
-        <v>95.2</v>
+        <v>89</v>
       </c>
       <c r="M10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O10">
-        <v>93.40000000000001</v>
+        <v>91.59999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C11">
-        <v>88.8</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="D11">
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
       <c r="E11">
-        <v>88.90000000000001</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="F11">
-        <v>3.9</v>
+        <v>0.4</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="I11">
-        <v>84.90000000000001</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="K11">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="L11">
-        <v>90.8</v>
+        <v>95.8</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N11">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O11">
-        <v>90.90000000000001</v>
+        <v>95.40000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B12">
-        <v>94.3</v>
+        <v>88.7</v>
       </c>
       <c r="C12">
-        <v>88.90000000000001</v>
+        <v>89.3</v>
       </c>
       <c r="D12">
-        <v>-5.4</v>
+        <v>0.6</v>
       </c>
       <c r="E12">
-        <v>89</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="F12">
-        <v>-5.3</v>
+        <v>0.8</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H12">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I12">
-        <v>92.90000000000001</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K12">
         <v>88</v>
       </c>
       <c r="L12">
-        <v>87.2</v>
+        <v>87</v>
       </c>
       <c r="M12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N12">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="O12">
-        <v>87</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B13">
-        <v>88.7</v>
+        <v>90.3</v>
       </c>
       <c r="C13">
-        <v>89.3</v>
+        <v>89.8</v>
       </c>
       <c r="D13">
-        <v>0.6</v>
+        <v>-0.6</v>
       </c>
       <c r="E13">
-        <v>89.5</v>
+        <v>90</v>
       </c>
       <c r="F13">
-        <v>0.8</v>
+        <v>-0.3</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H13">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I13">
-        <v>95.8</v>
+        <v>93.7</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L13">
-        <v>86.7</v>
+        <v>84.8</v>
       </c>
       <c r="M13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N13">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="O13">
-        <v>86</v>
+        <v>91.40000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B14">
-        <v>92.7</v>
+        <v>90.7</v>
       </c>
       <c r="C14">
-        <v>89.3</v>
+        <v>90.2</v>
       </c>
       <c r="D14">
-        <v>-3.3</v>
+        <v>-0.5</v>
       </c>
       <c r="E14">
-        <v>89.5</v>
+        <v>90.5</v>
       </c>
       <c r="F14">
-        <v>-3.2</v>
+        <v>-0.2</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H14">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I14">
-        <v>92.5</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K14">
+        <v>96</v>
+      </c>
+      <c r="L14">
+        <v>93</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14">
         <v>94</v>
       </c>
-      <c r="L14">
-        <v>89</v>
-      </c>
-      <c r="M14" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14">
-        <v>92</v>
-      </c>
       <c r="O14">
-        <v>86.90000000000001</v>
+        <v>91.3</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B15">
-        <v>90.3</v>
+        <v>94.3</v>
       </c>
       <c r="C15">
-        <v>89.7</v>
+        <v>90.5</v>
       </c>
       <c r="D15">
-        <v>-0.6</v>
+        <v>-3.9</v>
       </c>
       <c r="E15">
-        <v>89.90000000000001</v>
+        <v>90.8</v>
       </c>
       <c r="F15">
-        <v>-0.5</v>
+        <v>-3.5</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I15">
-        <v>95.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="J15" t="s">
         <v>35</v>
       </c>
       <c r="K15">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L15">
-        <v>84.2</v>
+        <v>87.8</v>
       </c>
       <c r="M15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N15">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O15">
-        <v>89.40000000000001</v>
+        <v>89.59999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B16">
-        <v>90.7</v>
+        <v>92.7</v>
       </c>
       <c r="C16">
-        <v>89.7</v>
+        <v>90.5</v>
       </c>
       <c r="D16">
-        <v>-0.9</v>
+        <v>-2.1</v>
       </c>
       <c r="E16">
-        <v>89.90000000000001</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="F16">
-        <v>-0.8</v>
+        <v>-1.8</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H16">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="I16">
-        <v>88.8</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16">
+        <v>94</v>
+      </c>
+      <c r="L16">
+        <v>91.2</v>
+      </c>
+      <c r="M16" t="s">
         <v>40</v>
       </c>
-      <c r="K16">
-        <v>96</v>
-      </c>
-      <c r="L16">
-        <v>90.90000000000001</v>
-      </c>
-      <c r="M16" t="s">
-        <v>38</v>
-      </c>
       <c r="N16">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O16">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B17">
-        <v>93.7</v>
+        <v>89.3</v>
       </c>
       <c r="C17">
-        <v>91.90000000000001</v>
+        <v>91.2</v>
       </c>
       <c r="D17">
-        <v>-1.8</v>
+        <v>1.8</v>
       </c>
       <c r="E17">
-        <v>92.40000000000001</v>
+        <v>91.5</v>
       </c>
       <c r="F17">
-        <v>-1.3</v>
+        <v>2.2</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H17">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I17">
-        <v>91.90000000000001</v>
+        <v>91.5</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K17">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="L17">
-        <v>97.59999999999999</v>
+        <v>82.7</v>
       </c>
       <c r="M17" t="s">
         <v>34</v>
       </c>
       <c r="N17">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="O17">
-        <v>87.5</v>
+        <v>100.4</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B18">
-        <v>89.3</v>
+        <v>89</v>
       </c>
       <c r="C18">
+        <v>92</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
         <v>92.40000000000001</v>
       </c>
-      <c r="D18">
-        <v>3.1</v>
-      </c>
-      <c r="E18">
-        <v>92.90000000000001</v>
-      </c>
       <c r="F18">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>89</v>
       </c>
       <c r="I18">
-        <v>93.3</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
         <v>29</v>
       </c>
       <c r="K18">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="L18">
-        <v>84.90000000000001</v>
+        <v>89.7</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N18">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="O18">
-        <v>100.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B19">
-        <v>93.3</v>
+        <v>93.7</v>
       </c>
       <c r="C19">
-        <v>92.5</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="D19">
-        <v>-0.8</v>
+        <v>-1.3</v>
       </c>
       <c r="E19">
         <v>93</v>
       </c>
       <c r="F19">
-        <v>-0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H19">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="I19">
-        <v>94.3</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K19">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L19">
-        <v>91.7</v>
+        <v>97.59999999999999</v>
       </c>
       <c r="M19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N19">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="O19">
-        <v>93</v>
+        <v>87.40000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B20">
         <v>93.3</v>
       </c>
       <c r="C20">
-        <v>92.7</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="D20">
-        <v>-0.6</v>
+        <v>-0.9</v>
       </c>
       <c r="E20">
-        <v>93.2</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="F20">
-        <v>-0.1</v>
+        <v>-0.4</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H20">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I20">
-        <v>96.2</v>
+        <v>92.5</v>
       </c>
       <c r="J20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K20">
+        <v>93</v>
+      </c>
+      <c r="L20">
         <v>92</v>
       </c>
-      <c r="L20">
-        <v>92.59999999999999</v>
-      </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N20">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="O20">
-        <v>90.90000000000001</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B21">
-        <v>93.7</v>
+        <v>93.3</v>
       </c>
       <c r="C21">
-        <v>93</v>
+        <v>92.7</v>
       </c>
       <c r="D21">
         <v>-0.7</v>
       </c>
       <c r="E21">
-        <v>93.5</v>
+        <v>93.2</v>
       </c>
       <c r="F21">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H21">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="I21">
-        <v>94.90000000000001</v>
+        <v>95.5</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K21">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L21">
-        <v>94.7</v>
+        <v>92.59999999999999</v>
       </c>
       <c r="M21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N21">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O21">
-        <v>91</v>
+        <v>91.59999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B22">
-        <v>89</v>
+        <v>93.7</v>
       </c>
       <c r="C22">
+        <v>93</v>
+      </c>
+      <c r="D22">
+        <v>-0.7</v>
+      </c>
+      <c r="E22">
+        <v>93.59999999999999</v>
+      </c>
+      <c r="F22">
+        <v>-0.1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <v>90</v>
+      </c>
+      <c r="I22">
         <v>93.40000000000001</v>
       </c>
-      <c r="D22">
-        <v>4.4</v>
-      </c>
-      <c r="E22">
-        <v>94</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22">
-        <v>89</v>
-      </c>
-      <c r="I22">
-        <v>96.8</v>
-      </c>
       <c r="J22" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K22">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="L22">
-        <v>91.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="M22" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="N22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="O22">
-        <v>93.2</v>
+        <v>92.3</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3115,16 +3115,16 @@
         <v>94</v>
       </c>
       <c r="C23">
-        <v>93.5</v>
+        <v>93.7</v>
       </c>
       <c r="D23">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="E23">
-        <v>94.2</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="F23">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -3133,7 +3133,7 @@
         <v>89</v>
       </c>
       <c r="I23">
-        <v>95.8</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="J23" t="s">
         <v>39</v>
@@ -3142,7 +3142,7 @@
         <v>97</v>
       </c>
       <c r="L23">
-        <v>92</v>
+        <v>94.2</v>
       </c>
       <c r="M23" t="s">
         <v>36</v>
@@ -3151,7 +3151,7 @@
         <v>96</v>
       </c>
       <c r="O23">
-        <v>94.7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -3162,16 +3162,16 @@
         <v>97</v>
       </c>
       <c r="C24">
-        <v>98.09999999999999</v>
+        <v>97.3</v>
       </c>
       <c r="D24">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="E24">
-        <v>99.2</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="F24">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="G24" t="s">
         <v>30</v>
@@ -3180,16 +3180,16 @@
         <v>97</v>
       </c>
       <c r="I24">
-        <v>101.9</v>
+        <v>100.4</v>
       </c>
       <c r="J24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K24">
         <v>94</v>
       </c>
       <c r="L24">
-        <v>95.2</v>
+        <v>94.5</v>
       </c>
       <c r="M24" t="s">
         <v>34</v>
@@ -3198,7 +3198,7 @@
         <v>100</v>
       </c>
       <c r="O24">
-        <v>100.5</v>
+        <v>100.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>